<commit_message>
Update code for more options
</commit_message>
<xml_diff>
--- a/Data/collected_stats.xlsx
+++ b/Data/collected_stats.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\UASeniorYear\ECE462\project\delivery\ECE462-FinalProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6833BB3-C796-4F7C-BA07-353CD4E77330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064678E3-DC62-474E-94F5-6223BD0BCE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23670" yWindow="2010" windowWidth="22455" windowHeight="12090" xr2:uid="{34DB9A80-D916-4322-B00C-A9A816055EC6}"/>
+    <workbookView xWindow="6848" yWindow="840" windowWidth="12509" windowHeight="10125" xr2:uid="{34DB9A80-D916-4322-B00C-A9A816055EC6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Default" sheetId="1" r:id="rId1"/>
+    <sheet name="CacheVariants" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="53">
   <si>
     <t>Uncached</t>
   </si>
@@ -82,9 +83,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Cached</t>
-  </si>
-  <si>
     <t>Fib</t>
   </si>
   <si>
@@ -103,9 +101,6 @@
     <t>First Rise</t>
   </si>
   <si>
-    <t>Smaller Mem, 16 sets</t>
-  </si>
-  <si>
     <t>Instruction Cache Only (16 sets)</t>
   </si>
   <si>
@@ -145,9 +140,6 @@
     <t>No cache</t>
   </si>
   <si>
-    <t>Code used: power</t>
-  </si>
-  <si>
     <t>Synthesis</t>
   </si>
   <si>
@@ -158,6 +150,51 @@
   </si>
   <si>
     <t>Hardware Utilization</t>
+  </si>
+  <si>
+    <t>Cached (16 sets)</t>
+  </si>
+  <si>
+    <t>32 sets</t>
+  </si>
+  <si>
+    <t>16 sets</t>
+  </si>
+  <si>
+    <t>8 sets</t>
+  </si>
+  <si>
+    <t>Block size = 4</t>
+  </si>
+  <si>
+    <t>Number sets = 16</t>
+  </si>
+  <si>
+    <t>Block size = 8</t>
+  </si>
+  <si>
+    <t>Block size = 2</t>
+  </si>
+  <si>
+    <t>Default from last sheet is</t>
+  </si>
+  <si>
+    <t>ADDR_SIZE=12</t>
+  </si>
+  <si>
+    <t>CACHE_SETS=16</t>
+  </si>
+  <si>
+    <t>LINE_WORDS=4</t>
+  </si>
+  <si>
+    <t>MEM_BLOCKS=256</t>
+  </si>
+  <si>
+    <t>Code: Power</t>
+  </si>
+  <si>
+    <t>Code: VBMSE</t>
   </si>
 </sst>
 </file>
@@ -520,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3767FE9-D88E-414D-8716-68C14776CE10}">
   <dimension ref="B2:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -577,12 +614,12 @@
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -603,7 +640,7 @@
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.45">
@@ -628,22 +665,19 @@
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
         <v>0</v>
       </c>
       <c r="J15" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" t="s">
         <v>23</v>
       </c>
-      <c r="N15" t="s">
-        <v>25</v>
-      </c>
       <c r="R15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.45">
@@ -680,7 +714,7 @@
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <v>11756310</v>
@@ -690,7 +724,7 @@
         <v>587814</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17">
         <v>65697550</v>
@@ -700,7 +734,7 @@
         <v>3284876</v>
       </c>
       <c r="J17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K17">
         <v>22802650</v>
@@ -710,7 +744,7 @@
         <v>1140131</v>
       </c>
       <c r="N17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O17">
         <v>65726390</v>
@@ -720,7 +754,7 @@
         <v>3286318</v>
       </c>
       <c r="R17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S17">
         <v>637870</v>
@@ -732,7 +766,7 @@
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <v>21170</v>
@@ -742,7 +776,7 @@
         <v>1057</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18">
         <v>480010</v>
@@ -752,7 +786,7 @@
         <v>23999</v>
       </c>
       <c r="J18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K18">
         <v>21170</v>
@@ -762,7 +796,7 @@
         <v>1057</v>
       </c>
       <c r="N18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O18">
         <v>480010</v>
@@ -772,7 +806,7 @@
         <v>23999</v>
       </c>
       <c r="R18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S18">
         <v>4690</v>
@@ -784,7 +818,7 @@
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19">
         <v>322090</v>
@@ -794,7 +828,7 @@
         <v>16103</v>
       </c>
       <c r="F19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G19">
         <v>12743190</v>
@@ -804,7 +838,7 @@
         <v>637158</v>
       </c>
       <c r="J19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K19">
         <v>1798890</v>
@@ -814,7 +848,7 @@
         <v>89943</v>
       </c>
       <c r="N19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O19">
         <v>12765850</v>
@@ -824,7 +858,7 @@
         <v>638291</v>
       </c>
       <c r="R19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S19">
         <v>123750</v>
@@ -836,7 +870,7 @@
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>2616810</v>
@@ -846,7 +880,7 @@
         <v>130839</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G20">
         <v>203396190</v>
@@ -856,7 +890,7 @@
         <v>10169808</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K20">
         <v>14550790</v>
@@ -866,7 +900,7 @@
         <v>727538</v>
       </c>
       <c r="N20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O20">
         <v>203828790</v>
@@ -876,7 +910,7 @@
         <v>10191438</v>
       </c>
       <c r="R20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S20">
         <v>1974750</v>
@@ -888,34 +922,53 @@
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B23" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F24" t="s">
-        <v>36</v>
+        <v>51</v>
+      </c>
+      <c r="I24" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L24" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>2062</v>
@@ -926,10 +979,22 @@
       <c r="E26">
         <v>63400</v>
       </c>
+      <c r="H26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26">
+        <v>14425</v>
+      </c>
+      <c r="J26">
+        <v>12346</v>
+      </c>
+      <c r="K26">
+        <v>63400</v>
+      </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>1614</v>
@@ -940,10 +1005,22 @@
       <c r="E27">
         <v>126800</v>
       </c>
+      <c r="H27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27">
+        <v>8823</v>
+      </c>
+      <c r="J27">
+        <v>496</v>
+      </c>
+      <c r="K27">
+        <v>126800</v>
+      </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -954,10 +1031,22 @@
       <c r="E28">
         <v>135</v>
       </c>
+      <c r="H28" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>135</v>
+      </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>7</v>
@@ -968,10 +1057,22 @@
       <c r="E29">
         <v>240</v>
       </c>
+      <c r="H29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29">
+        <v>7</v>
+      </c>
+      <c r="J29">
+        <v>7</v>
+      </c>
+      <c r="K29">
+        <v>240</v>
+      </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>130</v>
@@ -982,10 +1083,22 @@
       <c r="E30">
         <v>210</v>
       </c>
+      <c r="H30" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30">
+        <v>130</v>
+      </c>
+      <c r="J30">
+        <v>130</v>
+      </c>
+      <c r="K30">
+        <v>210</v>
+      </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -996,13 +1109,28 @@
       <c r="E31">
         <v>32</v>
       </c>
+      <c r="H31" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31">
+        <v>12</v>
+      </c>
+      <c r="J31">
+        <v>12</v>
+      </c>
+      <c r="K31">
+        <v>32</v>
+      </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.45">
       <c r="C32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+      <c r="I32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C33">
         <v>2057</v>
       </c>
@@ -1012,8 +1140,17 @@
       <c r="E33">
         <v>63400</v>
       </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="I33">
+        <v>14415</v>
+      </c>
+      <c r="J33">
+        <v>12341</v>
+      </c>
+      <c r="K33">
+        <v>63400</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C34">
         <v>1614</v>
       </c>
@@ -1023,8 +1160,17 @@
       <c r="E34">
         <v>126800</v>
       </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="I34">
+        <v>8823</v>
+      </c>
+      <c r="J34">
+        <v>496</v>
+      </c>
+      <c r="K34">
+        <v>126800</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C35">
         <v>1</v>
       </c>
@@ -1034,8 +1180,17 @@
       <c r="E35">
         <v>135</v>
       </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C36">
         <v>7</v>
       </c>
@@ -1045,8 +1200,17 @@
       <c r="E36">
         <v>240</v>
       </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="I36">
+        <v>7</v>
+      </c>
+      <c r="J36">
+        <v>7</v>
+      </c>
+      <c r="K36">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C37">
         <v>130</v>
       </c>
@@ -1056,8 +1220,17 @@
       <c r="E37">
         <v>210</v>
       </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="I37">
+        <v>130</v>
+      </c>
+      <c r="J37">
+        <v>130</v>
+      </c>
+      <c r="K37">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C38">
         <v>1</v>
       </c>
@@ -1065,6 +1238,15 @@
         <v>1</v>
       </c>
       <c r="E38">
+        <v>32</v>
+      </c>
+      <c r="I38">
+        <v>12</v>
+      </c>
+      <c r="J38">
+        <v>12</v>
+      </c>
+      <c r="K38">
         <v>32</v>
       </c>
     </row>
@@ -1072,4 +1254,424 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4D256E-8FE7-4149-9C2C-22CDC97BF1E9}">
+  <dimension ref="B4:L27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="18.53125" customWidth="1"/>
+    <col min="6" max="6" width="18.73046875" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <f>2*10</f>
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>11756310</v>
+      </c>
+      <c r="D17">
+        <f>(C17-$H$13)/$D$12</f>
+        <v>587814</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17">
+        <v>11756310</v>
+      </c>
+      <c r="H17">
+        <f>(G17-$H$13)/$D$12</f>
+        <v>587814</v>
+      </c>
+      <c r="J17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17">
+        <v>11756310</v>
+      </c>
+      <c r="L17">
+        <f>(K17-$H$13)/$D$12</f>
+        <v>587814</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>21170</v>
+      </c>
+      <c r="D18">
+        <f>(C18-$H$13)/$D$12</f>
+        <v>1057</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18">
+        <v>21170</v>
+      </c>
+      <c r="H18">
+        <f>(G18-$H$13)/$D$12</f>
+        <v>1057</v>
+      </c>
+      <c r="J18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18">
+        <v>21170</v>
+      </c>
+      <c r="L18">
+        <f>(K18-$H$13)/$D$12</f>
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>322090</v>
+      </c>
+      <c r="D19">
+        <f>(C19-$H$13)/$D$12</f>
+        <v>16103</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19">
+        <v>322090</v>
+      </c>
+      <c r="H19">
+        <f>(G19-$H$13)/$D$12</f>
+        <v>16103</v>
+      </c>
+      <c r="J19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19">
+        <v>322090</v>
+      </c>
+      <c r="L19">
+        <f>(K19-$H$13)/$D$12</f>
+        <v>16103</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>2349010</v>
+      </c>
+      <c r="D20">
+        <f>(C20-$H$13)/$D$12</f>
+        <v>117449</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20">
+        <v>2616810</v>
+      </c>
+      <c r="H20">
+        <f>(G20-$H$13)/$D$12</f>
+        <v>130839</v>
+      </c>
+      <c r="J20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20">
+        <v>10790890</v>
+      </c>
+      <c r="L20">
+        <f>(K20-$H$13)/$D$12</f>
+        <v>539543</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>11733650</v>
+      </c>
+      <c r="D24">
+        <f>(C24-$H$13)/$D$12</f>
+        <v>586681</v>
+      </c>
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24">
+        <v>11756310</v>
+      </c>
+      <c r="H24">
+        <f>(G24-$H$13)/$D$12</f>
+        <v>587814</v>
+      </c>
+      <c r="J24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24">
+        <v>11801630</v>
+      </c>
+      <c r="L24">
+        <f>(K24-$H$13)/$D$12</f>
+        <v>590080</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>12930</v>
+      </c>
+      <c r="D25">
+        <f>(C25-$H$13)/$D$12</f>
+        <v>645</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25">
+        <v>21170</v>
+      </c>
+      <c r="H25">
+        <f>(G25-$H$13)/$D$12</f>
+        <v>1057</v>
+      </c>
+      <c r="J25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25">
+        <v>37650</v>
+      </c>
+      <c r="L25">
+        <f>(K25-$H$13)/$D$12</f>
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>301490</v>
+      </c>
+      <c r="D26">
+        <f>(C26-$H$13)/$D$12</f>
+        <v>15073</v>
+      </c>
+      <c r="F26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26">
+        <v>322090</v>
+      </c>
+      <c r="H26">
+        <f>(G26-$H$13)/$D$12</f>
+        <v>16103</v>
+      </c>
+      <c r="J26" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26">
+        <v>369470</v>
+      </c>
+      <c r="L26">
+        <f>(K26-$H$13)/$D$12</f>
+        <v>18472</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>2206870</v>
+      </c>
+      <c r="D27">
+        <f>(C27-$H$13)/$D$12</f>
+        <v>110342</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27">
+        <v>2616810</v>
+      </c>
+      <c r="H27">
+        <f>(G27-$H$13)/$D$12</f>
+        <v>130839</v>
+      </c>
+      <c r="J27" t="s">
+        <v>18</v>
+      </c>
+      <c r="K27">
+        <v>13952990</v>
+      </c>
+      <c r="L27">
+        <f>(K27-$H$13)/$D$12</f>
+        <v>697648</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>